<commit_message>
Excel update + Change NavigateDate
</commit_message>
<xml_diff>
--- a/data/VM_BetDraft.xlsx
+++ b/data/VM_BetDraft.xlsx
@@ -1,27 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nygard001\VM2018\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklas/Development/VM2018/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE263C9A-55C4-EF43-A5C8-ACFF918A4C21}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="465" windowWidth="16125" windowHeight="16380"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="179017"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1092" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="99">
   <si>
     <t>Resultat</t>
   </si>
@@ -323,7 +324,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1086,14 +1087,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
-    <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
-    <cellStyle name="20% - Accent5" xfId="8" builtinId="46"/>
-    <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
-    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
-    <cellStyle name="40% - Accent3" xfId="5" builtinId="39"/>
-    <cellStyle name="40% - Accent4" xfId="4" builtinId="43"/>
-    <cellStyle name="Input" xfId="7" builtinId="20"/>
+    <cellStyle name="20 % - Dekorfärg1" xfId="1" builtinId="30"/>
+    <cellStyle name="20 % - Dekorfärg4" xfId="3" builtinId="42"/>
+    <cellStyle name="20 % - Dekorfärg5" xfId="8" builtinId="46"/>
+    <cellStyle name="40 % - Dekorfärg1" xfId="2" builtinId="31"/>
+    <cellStyle name="40 % - Dekorfärg2" xfId="6" builtinId="35"/>
+    <cellStyle name="40 % - Dekorfärg3" xfId="5" builtinId="39"/>
+    <cellStyle name="40 % - Dekorfärg4" xfId="4" builtinId="43"/>
+    <cellStyle name="Indata" xfId="7" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1110,7 +1111,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1405,36 +1406,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AL836"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="K70" sqref="K70"/>
+    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
+      <selection activeCell="AI62" sqref="AI62:AJ63"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.42578125" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="12.42578125" customWidth="1"/>
-    <col min="6" max="10" width="8.7109375" customWidth="1"/>
-    <col min="11" max="11" width="8.7109375" style="12" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" style="54" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="14.85546875" style="12" customWidth="1"/>
-    <col min="15" max="15" width="8.7109375" customWidth="1"/>
-    <col min="16" max="16" width="14.42578125" style="54" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="14.42578125" style="54" customWidth="1"/>
+    <col min="1" max="2" width="12.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.5" customWidth="1"/>
+    <col min="4" max="4" width="12.5" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.5" customWidth="1"/>
+    <col min="6" max="10" width="8.6640625" customWidth="1"/>
+    <col min="11" max="11" width="8.6640625" style="12" customWidth="1"/>
+    <col min="12" max="12" width="14.83203125" style="54" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.83203125" style="12" customWidth="1"/>
+    <col min="15" max="15" width="8.6640625" customWidth="1"/>
+    <col min="16" max="16" width="14.5" style="54" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="14.5" style="54" customWidth="1"/>
     <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.42578125" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="16.42578125" customWidth="1"/>
-    <col min="24" max="26" width="14.42578125" style="64"/>
-    <col min="28" max="30" width="14.42578125" style="64"/>
-    <col min="32" max="34" width="14.42578125" style="64"/>
-    <col min="36" max="38" width="14.42578125" style="64"/>
+    <col min="20" max="20" width="16.5" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="16.5" customWidth="1"/>
+    <col min="24" max="26" width="14.5" style="64"/>
+    <col min="28" max="30" width="14.5" style="64"/>
+    <col min="32" max="34" width="14.5" style="64"/>
+    <col min="36" max="38" width="14.5" style="64"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" s="26" t="s">
         <v>60</v>
       </c>
@@ -1571,7 +1572,7 @@
         <v>Philip_Borta</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
@@ -1661,7 +1662,7 @@
       <c r="AK2" s="46"/>
       <c r="AL2" s="46"/>
     </row>
-    <row r="3" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:38" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="39" t="s">
         <v>11</v>
       </c>
@@ -1751,7 +1752,7 @@
       <c r="AK3" s="46"/>
       <c r="AL3" s="46"/>
     </row>
-    <row r="4" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:38" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="39" t="s">
         <v>15</v>
       </c>
@@ -1841,7 +1842,7 @@
       <c r="AK4" s="46"/>
       <c r="AL4" s="46"/>
     </row>
-    <row r="5" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:38" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="39" t="s">
         <v>13</v>
       </c>
@@ -1931,7 +1932,7 @@
       <c r="AK5" s="46"/>
       <c r="AL5" s="46"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
@@ -2021,7 +2022,7 @@
       <c r="AK6" s="46"/>
       <c r="AL6" s="46"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>21</v>
       </c>
@@ -2111,7 +2112,7 @@
       <c r="AK7" s="46"/>
       <c r="AL7" s="46"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2201,7 +2202,7 @@
       <c r="AK8" s="46"/>
       <c r="AL8" s="46"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
@@ -2291,7 +2292,7 @@
       <c r="AK9" s="46"/>
       <c r="AL9" s="46"/>
     </row>
-    <row r="10" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:38" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="39" t="s">
         <v>29</v>
       </c>
@@ -2381,7 +2382,7 @@
       <c r="AK10" s="46"/>
       <c r="AL10" s="46"/>
     </row>
-    <row r="11" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:38" ht="16" x14ac:dyDescent="0.2">
       <c r="A11" s="39" t="s">
         <v>25</v>
       </c>
@@ -2471,7 +2472,7 @@
       <c r="AK11" s="46"/>
       <c r="AL11" s="46"/>
     </row>
-    <row r="12" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:38" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="39" t="s">
         <v>27</v>
       </c>
@@ -2561,7 +2562,7 @@
       <c r="AK12" s="46"/>
       <c r="AL12" s="46"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A13" s="9" t="s">
         <v>31</v>
       </c>
@@ -2651,7 +2652,7 @@
       <c r="AK13" s="46"/>
       <c r="AL13" s="46"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A14" s="9" t="s">
         <v>33</v>
       </c>
@@ -2741,7 +2742,7 @@
       <c r="AK14" s="46"/>
       <c r="AL14" s="46"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
       <c r="A15" s="9" t="s">
         <v>35</v>
       </c>
@@ -2831,7 +2832,7 @@
       <c r="AK15" s="46"/>
       <c r="AL15" s="46"/>
     </row>
-    <row r="16" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:38" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="39" t="s">
         <v>39</v>
       </c>
@@ -2921,7 +2922,7 @@
       <c r="AK16" s="46"/>
       <c r="AL16" s="46"/>
     </row>
-    <row r="17" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:38" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="39" t="s">
         <v>37</v>
       </c>
@@ -3011,7 +3012,7 @@
       <c r="AK17" s="46"/>
       <c r="AL17" s="46"/>
     </row>
-    <row r="18" spans="1:38" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:38" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="56" t="s">
         <v>9</v>
       </c>
@@ -3101,7 +3102,7 @@
       <c r="AK18" s="62"/>
       <c r="AL18" s="62"/>
     </row>
-    <row r="19" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="11" t="s">
         <v>12</v>
       </c>
@@ -3191,7 +3192,7 @@
       <c r="AK19" s="46"/>
       <c r="AL19" s="46"/>
     </row>
-    <row r="20" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -3281,7 +3282,7 @@
       <c r="AK20" s="46"/>
       <c r="AL20" s="46"/>
     </row>
-    <row r="21" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>41</v>
       </c>
@@ -3371,7 +3372,7 @@
       <c r="AK21" s="46"/>
       <c r="AL21" s="46"/>
     </row>
-    <row r="22" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="39" t="s">
         <v>17</v>
       </c>
@@ -3461,7 +3462,7 @@
       <c r="AK22" s="46"/>
       <c r="AL22" s="46"/>
     </row>
-    <row r="23" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -3551,7 +3552,7 @@
       <c r="AK23" s="46"/>
       <c r="AL23" s="46"/>
     </row>
-    <row r="24" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="39" t="s">
         <v>19</v>
       </c>
@@ -3641,7 +3642,7 @@
       <c r="AK24" s="46"/>
       <c r="AL24" s="46"/>
     </row>
-    <row r="25" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>24</v>
       </c>
@@ -3731,7 +3732,7 @@
       <c r="AK25" s="46"/>
       <c r="AL25" s="46"/>
     </row>
-    <row r="26" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
@@ -3821,7 +3822,7 @@
       <c r="AK26" s="46"/>
       <c r="AL26" s="46"/>
     </row>
-    <row r="27" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>26</v>
       </c>
@@ -3911,7 +3912,7 @@
       <c r="AK27" s="46"/>
       <c r="AL27" s="46"/>
     </row>
-    <row r="28" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="39" t="s">
         <v>27</v>
       </c>
@@ -4001,7 +4002,7 @@
       <c r="AK28" s="46"/>
       <c r="AL28" s="46"/>
     </row>
-    <row r="29" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="39" t="s">
         <v>32</v>
       </c>
@@ -4091,7 +4092,7 @@
       <c r="AK29" s="46"/>
       <c r="AL29" s="46"/>
     </row>
-    <row r="30" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="39" t="s">
         <v>42</v>
       </c>
@@ -4181,7 +4182,7 @@
       <c r="AK30" s="46"/>
       <c r="AL30" s="46"/>
     </row>
-    <row r="31" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>36</v>
       </c>
@@ -4271,7 +4272,7 @@
       <c r="AK31" s="46"/>
       <c r="AL31" s="46"/>
     </row>
-    <row r="32" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>43</v>
       </c>
@@ -4361,7 +4362,7 @@
       <c r="AK32" s="46"/>
       <c r="AL32" s="46"/>
     </row>
-    <row r="33" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>38</v>
       </c>
@@ -4451,7 +4452,7 @@
       <c r="AK33" s="46"/>
       <c r="AL33" s="46"/>
     </row>
-    <row r="34" spans="1:38" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:38" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="56" t="s">
         <v>12</v>
       </c>
@@ -4541,7 +4542,7 @@
       <c r="AK34" s="62"/>
       <c r="AL34" s="62"/>
     </row>
-    <row r="35" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="39" t="s">
         <v>10</v>
       </c>
@@ -4631,7 +4632,7 @@
       <c r="AK35" s="46"/>
       <c r="AL35" s="46"/>
     </row>
-    <row r="36" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="43" t="s">
         <v>14</v>
       </c>
@@ -4721,7 +4722,7 @@
       <c r="AK36" s="46"/>
       <c r="AL36" s="46"/>
     </row>
-    <row r="37" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="43" t="s">
         <v>16</v>
       </c>
@@ -4811,7 +4812,7 @@
       <c r="AK37" s="46"/>
       <c r="AL37" s="46"/>
     </row>
-    <row r="38" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>22</v>
       </c>
@@ -4901,7 +4902,7 @@
       <c r="AK38" s="46"/>
       <c r="AL38" s="46"/>
     </row>
-    <row r="39" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>18</v>
       </c>
@@ -4991,7 +4992,7 @@
       <c r="AK39" s="46"/>
       <c r="AL39" s="46"/>
     </row>
-    <row r="40" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A40" s="11" t="s">
         <v>44</v>
       </c>
@@ -5081,7 +5082,7 @@
       <c r="AK40" s="46"/>
       <c r="AL40" s="46"/>
     </row>
-    <row r="41" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="11" t="s">
         <v>20</v>
       </c>
@@ -5171,7 +5172,7 @@
       <c r="AK41" s="46"/>
       <c r="AL41" s="46"/>
     </row>
-    <row r="42" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A42" s="39" t="s">
         <v>47</v>
       </c>
@@ -5261,7 +5262,7 @@
       <c r="AK42" s="46"/>
       <c r="AL42" s="46"/>
     </row>
-    <row r="43" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A43" s="39" t="s">
         <v>48</v>
       </c>
@@ -5351,7 +5352,7 @@
       <c r="AK43" s="66"/>
       <c r="AL43" s="66"/>
     </row>
-    <row r="44" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="39" t="s">
         <v>46</v>
       </c>
@@ -5441,7 +5442,7 @@
       <c r="AK44" s="46"/>
       <c r="AL44" s="46"/>
     </row>
-    <row r="45" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A45" s="39" t="s">
         <v>45</v>
       </c>
@@ -5531,7 +5532,7 @@
       <c r="AK45" s="46"/>
       <c r="AL45" s="46"/>
     </row>
-    <row r="46" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>51</v>
       </c>
@@ -5621,7 +5622,7 @@
       <c r="AK46" s="46"/>
       <c r="AL46" s="46"/>
     </row>
-    <row r="47" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>52</v>
       </c>
@@ -5711,7 +5712,7 @@
       <c r="AK47" s="46"/>
       <c r="AL47" s="46"/>
     </row>
-    <row r="48" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>49</v>
       </c>
@@ -5801,7 +5802,7 @@
       <c r="AK48" s="46"/>
       <c r="AL48" s="46"/>
     </row>
-    <row r="49" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="73" t="s">
         <v>50</v>
       </c>
@@ -5891,7 +5892,7 @@
       <c r="AK49" s="46"/>
       <c r="AL49" s="46"/>
     </row>
-    <row r="50" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="88" t="s">
         <v>12</v>
       </c>
@@ -6003,7 +6004,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="87" t="s">
         <v>17</v>
       </c>
@@ -6111,7 +6112,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="87" t="s">
         <v>16</v>
       </c>
@@ -6219,7 +6220,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="87" t="s">
         <v>23</v>
       </c>
@@ -6331,7 +6332,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="87" t="s">
         <v>29</v>
       </c>
@@ -6443,7 +6444,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="87" t="s">
         <v>42</v>
       </c>
@@ -6555,7 +6556,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="87" t="s">
         <v>31</v>
       </c>
@@ -6667,7 +6668,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="87" t="s">
         <v>37</v>
       </c>
@@ -6779,7 +6780,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="94" t="s">
         <v>12</v>
       </c>
@@ -6891,7 +6892,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="84" t="s">
         <v>29</v>
       </c>
@@ -7003,7 +7004,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="84" t="s">
         <v>9</v>
       </c>
@@ -7115,7 +7116,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="84" t="s">
         <v>31</v>
       </c>
@@ -7227,7 +7228,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="104" t="s">
         <v>17</v>
       </c>
@@ -7254,56 +7255,84 @@
       </c>
       <c r="I62" s="92"/>
       <c r="J62" s="92"/>
-      <c r="K62" s="92"/>
-      <c r="L62" s="93"/>
+      <c r="K62" s="92">
+        <v>2</v>
+      </c>
+      <c r="L62" s="93" t="s">
+        <v>77</v>
+      </c>
       <c r="M62" s="94" t="s">
         <v>12</v>
       </c>
       <c r="N62" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="O62" s="92"/>
-      <c r="P62" s="95"/>
+      <c r="O62" s="92">
+        <v>2</v>
+      </c>
+      <c r="P62" s="95" t="s">
+        <v>78</v>
+      </c>
       <c r="Q62" s="94" t="s">
         <v>16</v>
       </c>
       <c r="R62" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="S62" s="92"/>
-      <c r="T62" s="93"/>
+      <c r="S62" s="92">
+        <v>2</v>
+      </c>
+      <c r="T62" s="93" t="s">
+        <v>78</v>
+      </c>
       <c r="U62" s="94" t="s">
         <v>17</v>
       </c>
       <c r="V62" s="94" t="s">
         <v>42</v>
       </c>
-      <c r="W62" s="92"/>
-      <c r="X62" s="95"/>
+      <c r="W62" s="92">
+        <v>1</v>
+      </c>
+      <c r="X62" s="95" t="s">
+        <v>69</v>
+      </c>
       <c r="Y62" s="94" t="s">
         <v>15</v>
       </c>
       <c r="Z62" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="AA62" s="92"/>
-      <c r="AB62" s="93"/>
+      <c r="AA62" s="92" t="s">
+        <v>8</v>
+      </c>
+      <c r="AB62" s="93" t="s">
+        <v>68</v>
+      </c>
       <c r="AC62" s="94" t="s">
         <v>12</v>
       </c>
       <c r="AD62" s="94" t="s">
         <v>19</v>
       </c>
-      <c r="AE62" s="92"/>
-      <c r="AF62" s="95"/>
+      <c r="AE62" s="92">
+        <v>2</v>
+      </c>
+      <c r="AF62" s="95" t="s">
+        <v>70</v>
+      </c>
       <c r="AG62" s="94" t="s">
         <v>12</v>
       </c>
       <c r="AH62" s="94" t="s">
         <v>29</v>
       </c>
-      <c r="AI62" s="92"/>
-      <c r="AJ62" s="93"/>
+      <c r="AI62" s="92">
+        <v>1</v>
+      </c>
+      <c r="AJ62" s="93" t="s">
+        <v>69</v>
+      </c>
       <c r="AK62" s="94" t="s">
         <v>17</v>
       </c>
@@ -7311,7 +7340,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="84" t="s">
         <v>23</v>
       </c>
@@ -7338,56 +7367,84 @@
       </c>
       <c r="I63" s="24"/>
       <c r="J63" s="24"/>
-      <c r="K63" s="16"/>
-      <c r="L63" s="46"/>
+      <c r="K63" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="L63" s="46" t="s">
+        <v>68</v>
+      </c>
       <c r="M63" s="82" t="s">
         <v>23</v>
       </c>
       <c r="N63" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="O63" s="19"/>
-      <c r="P63" s="81"/>
+      <c r="O63" s="19">
+        <v>1</v>
+      </c>
+      <c r="P63" s="81" t="s">
+        <v>69</v>
+      </c>
       <c r="Q63" s="83" t="s">
         <v>23</v>
       </c>
       <c r="R63" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="S63" s="16"/>
-      <c r="T63" s="46"/>
+      <c r="S63" s="16" t="s">
+        <v>58</v>
+      </c>
+      <c r="T63" s="46" t="s">
+        <v>67</v>
+      </c>
       <c r="U63" s="82" t="s">
         <v>15</v>
       </c>
       <c r="V63" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="W63" s="19"/>
-      <c r="X63" s="81"/>
+      <c r="W63" s="19">
+        <v>2</v>
+      </c>
+      <c r="X63" s="81" t="s">
+        <v>66</v>
+      </c>
       <c r="Y63" s="83" t="s">
         <v>12</v>
       </c>
       <c r="Z63" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="AA63" s="16"/>
-      <c r="AB63" s="85"/>
+      <c r="AA63" s="16">
+        <v>1</v>
+      </c>
+      <c r="AB63" s="85" t="s">
+        <v>69</v>
+      </c>
       <c r="AC63" s="86" t="s">
         <v>29</v>
       </c>
       <c r="AD63" s="86" t="s">
         <v>27</v>
       </c>
-      <c r="AE63" s="19"/>
-      <c r="AF63" s="81"/>
+      <c r="AE63" s="19" t="s">
+        <v>58</v>
+      </c>
+      <c r="AF63" s="81" t="s">
+        <v>67</v>
+      </c>
       <c r="AG63" s="83" t="s">
         <v>19</v>
       </c>
       <c r="AH63" s="83" t="s">
         <v>27</v>
       </c>
-      <c r="AI63" s="16"/>
-      <c r="AJ63" s="46"/>
+      <c r="AI63" s="16">
+        <v>1</v>
+      </c>
+      <c r="AJ63" s="46" t="s">
+        <v>69</v>
+      </c>
       <c r="AK63" s="82" t="s">
         <v>15</v>
       </c>
@@ -7395,7 +7452,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="94" t="s">
         <v>94</v>
       </c>
@@ -7473,7 +7530,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="84" t="s">
         <v>96</v>
       </c>
@@ -7551,777 +7608,777 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="67" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="68" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="69" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="70" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="71" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="72" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="73" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="74" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="75" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="76" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="77" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="78" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="79" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="80" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="66" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="67" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="68" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="69" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="70" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="71" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="72" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="73" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="74" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="75" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="76" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="77" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="78" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="79" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="80" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8332,16 +8389,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="C1" s="105" t="s">
         <v>55</v>
       </c>
@@ -8351,7 +8408,7 @@
       </c>
       <c r="F1" s="106"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8380,7 +8437,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
@@ -8420,7 +8477,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -8460,7 +8517,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
@@ -8500,7 +8557,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -8540,7 +8597,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>17</v>
       </c>
@@ -8580,7 +8637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
@@ -8620,7 +8677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
@@ -8660,7 +8717,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
@@ -8700,7 +8757,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>29</v>
       </c>
@@ -8740,7 +8797,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
@@ -8780,7 +8837,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>27</v>
       </c>
@@ -8820,7 +8877,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>31</v>
       </c>
@@ -8860,7 +8917,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>33</v>
       </c>
@@ -8900,7 +8957,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A16" s="9" t="s">
         <v>35</v>
       </c>
@@ -8940,7 +8997,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A17" s="11" t="s">
         <v>39</v>
       </c>
@@ -8980,7 +9037,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A18" s="11" t="s">
         <v>37</v>
       </c>
@@ -9020,7 +9077,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>9</v>
       </c>
@@ -9060,7 +9117,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>12</v>
       </c>
@@ -9100,7 +9157,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>15</v>
       </c>
@@ -9140,7 +9197,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>41</v>
       </c>
@@ -9180,7 +9237,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>17</v>
       </c>
@@ -9220,7 +9277,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>22</v>
       </c>
@@ -9260,7 +9317,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>19</v>
       </c>
@@ -9300,7 +9357,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>24</v>
       </c>
@@ -9340,7 +9397,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
@@ -9380,7 +9437,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>26</v>
       </c>
@@ -9420,7 +9477,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>27</v>
       </c>
@@ -9460,7 +9517,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>32</v>
       </c>
@@ -9500,7 +9557,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>42</v>
       </c>
@@ -9540,7 +9597,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>36</v>
       </c>
@@ -9580,7 +9637,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>43</v>
       </c>
@@ -9620,7 +9677,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>38</v>
       </c>
@@ -9660,7 +9717,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -9700,7 +9757,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>10</v>
       </c>
@@ -9740,7 +9797,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A37" s="9" t="s">
         <v>14</v>
       </c>
@@ -9780,7 +9837,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A38" s="9" t="s">
         <v>16</v>
       </c>
@@ -9820,7 +9877,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>22</v>
       </c>
@@ -9860,7 +9917,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>18</v>
       </c>
@@ -9900,7 +9957,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>44</v>
       </c>
@@ -9940,7 +9997,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>20</v>
       </c>
@@ -9980,7 +10037,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>47</v>
       </c>
@@ -10020,7 +10077,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>48</v>
       </c>
@@ -10060,7 +10117,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>46</v>
       </c>
@@ -10100,7 +10157,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>45</v>
       </c>
@@ -10140,7 +10197,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>51</v>
       </c>
@@ -10180,7 +10237,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>52</v>
       </c>
@@ -10220,7 +10277,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>49</v>
       </c>
@@ -10260,7 +10317,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>50</v>
       </c>
@@ -10310,7 +10367,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10320,9 +10377,9 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C3" t="s">
         <v>56</v>
       </c>
@@ -10330,12 +10387,12 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
       <c r="C5" s="4">
         <v>1</v>
       </c>
@@ -10349,7 +10406,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
@@ -10369,7 +10426,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
@@ -10389,7 +10446,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -10409,7 +10466,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A9" s="11" t="s">
         <v>13</v>
       </c>
@@ -10429,7 +10486,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
@@ -10449,7 +10506,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -10469,7 +10526,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
@@ -10489,7 +10546,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A13" s="11" t="s">
         <v>23</v>
       </c>
@@ -10511,7 +10568,7 @@
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A14" s="11" t="s">
         <v>29</v>
       </c>
@@ -10531,7 +10588,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
@@ -10551,7 +10608,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
@@ -10571,7 +10628,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A17" s="9" t="s">
         <v>31</v>
       </c>
@@ -10591,7 +10648,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A18" s="9" t="s">
         <v>33</v>
       </c>
@@ -10611,7 +10668,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A19" s="9" t="s">
         <v>35</v>
       </c>
@@ -10631,7 +10688,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A20" s="11" t="s">
         <v>39</v>
       </c>
@@ -10651,7 +10708,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A21" s="11" t="s">
         <v>37</v>
       </c>
@@ -10671,7 +10728,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
@@ -10691,7 +10748,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -10711,7 +10768,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A24" s="11" t="s">
         <v>15</v>
       </c>
@@ -10731,7 +10788,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A25" s="11" t="s">
         <v>41</v>
       </c>
@@ -10751,7 +10808,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A26" s="11" t="s">
         <v>17</v>
       </c>
@@ -10771,7 +10828,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A27" s="11" t="s">
         <v>22</v>
       </c>
@@ -10791,7 +10848,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -10811,7 +10868,7 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
@@ -10831,7 +10888,7 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A30" s="11" t="s">
         <v>29</v>
       </c>
@@ -10851,7 +10908,7 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A31" s="11" t="s">
         <v>26</v>
       </c>
@@ -10871,7 +10928,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A32" s="11" t="s">
         <v>27</v>
       </c>
@@ -10891,7 +10948,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A33" s="11" t="s">
         <v>32</v>
       </c>
@@ -10911,7 +10968,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A34" s="11" t="s">
         <v>42</v>
       </c>
@@ -10931,7 +10988,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A35" s="11" t="s">
         <v>36</v>
       </c>
@@ -10951,7 +11008,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A36" s="11" t="s">
         <v>43</v>
       </c>
@@ -10971,7 +11028,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A37" s="11" t="s">
         <v>38</v>
       </c>
@@ -10991,7 +11048,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A38" s="11" t="s">
         <v>12</v>
       </c>
@@ -11011,7 +11068,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A39" s="11" t="s">
         <v>10</v>
       </c>
@@ -11031,7 +11088,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A40" s="9" t="s">
         <v>14</v>
       </c>
@@ -11051,7 +11108,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A41" s="9" t="s">
         <v>16</v>
       </c>
@@ -11071,7 +11128,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A42" s="11" t="s">
         <v>22</v>
       </c>
@@ -11091,7 +11148,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A43" s="11" t="s">
         <v>18</v>
       </c>
@@ -11111,7 +11168,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A44" s="11" t="s">
         <v>44</v>
       </c>
@@ -11131,7 +11188,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="11" t="s">
         <v>20</v>
       </c>
@@ -11151,7 +11208,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A46" s="11" t="s">
         <v>47</v>
       </c>
@@ -11171,7 +11228,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A47" s="11" t="s">
         <v>48</v>
       </c>
@@ -11191,7 +11248,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A48" s="11" t="s">
         <v>46</v>
       </c>
@@ -11211,7 +11268,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A49" s="11" t="s">
         <v>45</v>
       </c>
@@ -11231,7 +11288,7 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A50" s="11" t="s">
         <v>51</v>
       </c>
@@ -11251,7 +11308,7 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
     </row>
-    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="11" t="s">
         <v>52</v>
       </c>
@@ -11268,7 +11325,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="11" t="s">
         <v>49</v>
       </c>
@@ -11285,7 +11342,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="11" t="s">
         <v>50</v>
       </c>

</xml_diff>

<commit_message>
Fix calculate score fulltime from if Score1et count goals < 91..........
</commit_message>
<xml_diff>
--- a/data/VM_BetDraft.xlsx
+++ b/data/VM_BetDraft.xlsx
@@ -1,28 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10523"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="18201"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/niklas/Development/VM2018/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nygard001\VM2018\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE263C9A-55C4-EF43-A5C8-ACFF918A4C21}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16380" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="465" windowWidth="28800" windowHeight="16380"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId2"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="179017"/>
+  <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1110" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1117" uniqueCount="95">
   <si>
     <t>Resultat</t>
   </si>
@@ -306,25 +305,13 @@
     <t>num</t>
   </si>
   <si>
-    <t>L 61</t>
-  </si>
-  <si>
-    <t>L 62</t>
-  </si>
-  <si>
-    <t>W 61</t>
-  </si>
-  <si>
-    <t>W 62</t>
-  </si>
-  <si>
     <t>2-5</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="14" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1087,14 +1074,14 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="9">
-    <cellStyle name="20 % - Dekorfärg1" xfId="1" builtinId="30"/>
-    <cellStyle name="20 % - Dekorfärg4" xfId="3" builtinId="42"/>
-    <cellStyle name="20 % - Dekorfärg5" xfId="8" builtinId="46"/>
-    <cellStyle name="40 % - Dekorfärg1" xfId="2" builtinId="31"/>
-    <cellStyle name="40 % - Dekorfärg2" xfId="6" builtinId="35"/>
-    <cellStyle name="40 % - Dekorfärg3" xfId="5" builtinId="39"/>
-    <cellStyle name="40 % - Dekorfärg4" xfId="4" builtinId="43"/>
-    <cellStyle name="Indata" xfId="7" builtinId="20"/>
+    <cellStyle name="20% - Accent1" xfId="1" builtinId="30"/>
+    <cellStyle name="20% - Accent4" xfId="3" builtinId="42"/>
+    <cellStyle name="20% - Accent5" xfId="8" builtinId="46"/>
+    <cellStyle name="40% - Accent1" xfId="2" builtinId="31"/>
+    <cellStyle name="40% - Accent2" xfId="6" builtinId="35"/>
+    <cellStyle name="40% - Accent3" xfId="5" builtinId="39"/>
+    <cellStyle name="40% - Accent4" xfId="4" builtinId="43"/>
+    <cellStyle name="Input" xfId="7" builtinId="20"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1111,7 +1098,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1406,36 +1393,36 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AL836"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A33" workbookViewId="0">
-      <selection activeCell="AI62" sqref="AI62:AJ63"/>
+    <sheetView tabSelected="1" topLeftCell="N49" workbookViewId="0">
+      <selection activeCell="X71" sqref="X71"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="12.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.5" customWidth="1"/>
-    <col min="4" max="4" width="12.5" style="7" customWidth="1"/>
-    <col min="5" max="5" width="12.5" customWidth="1"/>
-    <col min="6" max="10" width="8.6640625" customWidth="1"/>
-    <col min="11" max="11" width="8.6640625" style="12" customWidth="1"/>
-    <col min="12" max="12" width="14.83203125" style="54" bestFit="1" customWidth="1"/>
-    <col min="13" max="14" width="14.83203125" style="12" customWidth="1"/>
-    <col min="15" max="15" width="8.6640625" customWidth="1"/>
-    <col min="16" max="16" width="14.5" style="54" bestFit="1" customWidth="1"/>
-    <col min="17" max="18" width="14.5" style="54" customWidth="1"/>
+    <col min="1" max="2" width="12.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.42578125" customWidth="1"/>
+    <col min="4" max="4" width="12.42578125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="12.42578125" customWidth="1"/>
+    <col min="6" max="10" width="8.7109375" customWidth="1"/>
+    <col min="11" max="11" width="8.7109375" style="12" customWidth="1"/>
+    <col min="12" max="12" width="14.85546875" style="54" bestFit="1" customWidth="1"/>
+    <col min="13" max="14" width="14.85546875" style="12" customWidth="1"/>
+    <col min="15" max="15" width="8.7109375" customWidth="1"/>
+    <col min="16" max="16" width="14.42578125" style="54" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="14.42578125" style="54" customWidth="1"/>
     <col min="19" max="19" width="8" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="21" max="22" width="16.5" customWidth="1"/>
-    <col min="24" max="26" width="14.5" style="64"/>
-    <col min="28" max="30" width="14.5" style="64"/>
-    <col min="32" max="34" width="14.5" style="64"/>
-    <col min="36" max="38" width="14.5" style="64"/>
+    <col min="20" max="20" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="21" max="22" width="16.42578125" customWidth="1"/>
+    <col min="24" max="26" width="14.42578125" style="64"/>
+    <col min="28" max="30" width="14.42578125" style="64"/>
+    <col min="32" max="34" width="14.42578125" style="64"/>
+    <col min="36" max="38" width="14.42578125" style="64"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:38" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:38" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="26" t="s">
         <v>60</v>
       </c>
@@ -1572,7 +1559,7 @@
         <v>Philip_Borta</v>
       </c>
     </row>
-    <row r="2" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>9</v>
       </c>
@@ -1662,7 +1649,7 @@
       <c r="AK2" s="46"/>
       <c r="AL2" s="46"/>
     </row>
-    <row r="3" spans="1:38" ht="16" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A3" s="39" t="s">
         <v>11</v>
       </c>
@@ -1752,7 +1739,7 @@
       <c r="AK3" s="46"/>
       <c r="AL3" s="46"/>
     </row>
-    <row r="4" spans="1:38" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A4" s="39" t="s">
         <v>15</v>
       </c>
@@ -1842,7 +1829,7 @@
       <c r="AK4" s="46"/>
       <c r="AL4" s="46"/>
     </row>
-    <row r="5" spans="1:38" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A5" s="39" t="s">
         <v>13</v>
       </c>
@@ -1932,7 +1919,7 @@
       <c r="AK5" s="46"/>
       <c r="AL5" s="46"/>
     </row>
-    <row r="6" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>17</v>
       </c>
@@ -2022,7 +2009,7 @@
       <c r="AK6" s="46"/>
       <c r="AL6" s="46"/>
     </row>
-    <row r="7" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>21</v>
       </c>
@@ -2112,7 +2099,7 @@
       <c r="AK7" s="46"/>
       <c r="AL7" s="46"/>
     </row>
-    <row r="8" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>19</v>
       </c>
@@ -2202,7 +2189,7 @@
       <c r="AK8" s="46"/>
       <c r="AL8" s="46"/>
     </row>
-    <row r="9" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>23</v>
       </c>
@@ -2292,7 +2279,7 @@
       <c r="AK9" s="46"/>
       <c r="AL9" s="46"/>
     </row>
-    <row r="10" spans="1:38" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A10" s="39" t="s">
         <v>29</v>
       </c>
@@ -2382,7 +2369,7 @@
       <c r="AK10" s="46"/>
       <c r="AL10" s="46"/>
     </row>
-    <row r="11" spans="1:38" ht="16" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A11" s="39" t="s">
         <v>25</v>
       </c>
@@ -2472,7 +2459,7 @@
       <c r="AK11" s="46"/>
       <c r="AL11" s="46"/>
     </row>
-    <row r="12" spans="1:38" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A12" s="39" t="s">
         <v>27</v>
       </c>
@@ -2562,7 +2549,7 @@
       <c r="AK12" s="46"/>
       <c r="AL12" s="46"/>
     </row>
-    <row r="13" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A13" s="9" t="s">
         <v>31</v>
       </c>
@@ -2652,7 +2639,7 @@
       <c r="AK13" s="46"/>
       <c r="AL13" s="46"/>
     </row>
-    <row r="14" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A14" s="9" t="s">
         <v>33</v>
       </c>
@@ -2742,7 +2729,7 @@
       <c r="AK14" s="46"/>
       <c r="AL14" s="46"/>
     </row>
-    <row r="15" spans="1:38" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:38" x14ac:dyDescent="0.25">
       <c r="A15" s="9" t="s">
         <v>35</v>
       </c>
@@ -2832,7 +2819,7 @@
       <c r="AK15" s="46"/>
       <c r="AL15" s="46"/>
     </row>
-    <row r="16" spans="1:38" ht="16" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A16" s="39" t="s">
         <v>39</v>
       </c>
@@ -2922,7 +2909,7 @@
       <c r="AK16" s="46"/>
       <c r="AL16" s="46"/>
     </row>
-    <row r="17" spans="1:38" ht="16" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:38" ht="15.75" x14ac:dyDescent="0.25">
       <c r="A17" s="39" t="s">
         <v>37</v>
       </c>
@@ -3012,7 +2999,7 @@
       <c r="AK17" s="46"/>
       <c r="AL17" s="46"/>
     </row>
-    <row r="18" spans="1:38" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:38" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A18" s="56" t="s">
         <v>9</v>
       </c>
@@ -3102,7 +3089,7 @@
       <c r="AK18" s="62"/>
       <c r="AL18" s="62"/>
     </row>
-    <row r="19" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A19" s="11" t="s">
         <v>12</v>
       </c>
@@ -3192,7 +3179,7 @@
       <c r="AK19" s="46"/>
       <c r="AL19" s="46"/>
     </row>
-    <row r="20" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>15</v>
       </c>
@@ -3282,7 +3269,7 @@
       <c r="AK20" s="46"/>
       <c r="AL20" s="46"/>
     </row>
-    <row r="21" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>41</v>
       </c>
@@ -3372,7 +3359,7 @@
       <c r="AK21" s="46"/>
       <c r="AL21" s="46"/>
     </row>
-    <row r="22" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A22" s="39" t="s">
         <v>17</v>
       </c>
@@ -3462,7 +3449,7 @@
       <c r="AK22" s="46"/>
       <c r="AL22" s="46"/>
     </row>
-    <row r="23" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A23" s="39" t="s">
         <v>22</v>
       </c>
@@ -3552,7 +3539,7 @@
       <c r="AK23" s="46"/>
       <c r="AL23" s="46"/>
     </row>
-    <row r="24" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A24" s="39" t="s">
         <v>19</v>
       </c>
@@ -3642,7 +3629,7 @@
       <c r="AK24" s="46"/>
       <c r="AL24" s="46"/>
     </row>
-    <row r="25" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>24</v>
       </c>
@@ -3732,7 +3719,7 @@
       <c r="AK25" s="46"/>
       <c r="AL25" s="46"/>
     </row>
-    <row r="26" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>29</v>
       </c>
@@ -3822,7 +3809,7 @@
       <c r="AK26" s="46"/>
       <c r="AL26" s="46"/>
     </row>
-    <row r="27" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>26</v>
       </c>
@@ -3912,7 +3899,7 @@
       <c r="AK27" s="46"/>
       <c r="AL27" s="46"/>
     </row>
-    <row r="28" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="39" t="s">
         <v>27</v>
       </c>
@@ -4002,7 +3989,7 @@
       <c r="AK28" s="46"/>
       <c r="AL28" s="46"/>
     </row>
-    <row r="29" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A29" s="39" t="s">
         <v>32</v>
       </c>
@@ -4092,7 +4079,7 @@
       <c r="AK29" s="46"/>
       <c r="AL29" s="46"/>
     </row>
-    <row r="30" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A30" s="39" t="s">
         <v>42</v>
       </c>
@@ -4182,7 +4169,7 @@
       <c r="AK30" s="46"/>
       <c r="AL30" s="46"/>
     </row>
-    <row r="31" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>36</v>
       </c>
@@ -4272,7 +4259,7 @@
       <c r="AK31" s="46"/>
       <c r="AL31" s="46"/>
     </row>
-    <row r="32" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>43</v>
       </c>
@@ -4362,7 +4349,7 @@
       <c r="AK32" s="46"/>
       <c r="AL32" s="46"/>
     </row>
-    <row r="33" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>38</v>
       </c>
@@ -4452,7 +4439,7 @@
       <c r="AK33" s="46"/>
       <c r="AL33" s="46"/>
     </row>
-    <row r="34" spans="1:38" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:38" s="63" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="56" t="s">
         <v>12</v>
       </c>
@@ -4542,7 +4529,7 @@
       <c r="AK34" s="62"/>
       <c r="AL34" s="62"/>
     </row>
-    <row r="35" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="39" t="s">
         <v>10</v>
       </c>
@@ -4632,7 +4619,7 @@
       <c r="AK35" s="46"/>
       <c r="AL35" s="46"/>
     </row>
-    <row r="36" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A36" s="43" t="s">
         <v>14</v>
       </c>
@@ -4722,7 +4709,7 @@
       <c r="AK36" s="46"/>
       <c r="AL36" s="46"/>
     </row>
-    <row r="37" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="43" t="s">
         <v>16</v>
       </c>
@@ -4812,7 +4799,7 @@
       <c r="AK37" s="46"/>
       <c r="AL37" s="46"/>
     </row>
-    <row r="38" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>22</v>
       </c>
@@ -4902,7 +4889,7 @@
       <c r="AK38" s="46"/>
       <c r="AL38" s="46"/>
     </row>
-    <row r="39" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>18</v>
       </c>
@@ -4992,7 +4979,7 @@
       <c r="AK39" s="46"/>
       <c r="AL39" s="46"/>
     </row>
-    <row r="40" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A40" s="11" t="s">
         <v>44</v>
       </c>
@@ -5082,7 +5069,7 @@
       <c r="AK40" s="46"/>
       <c r="AL40" s="46"/>
     </row>
-    <row r="41" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A41" s="11" t="s">
         <v>20</v>
       </c>
@@ -5172,7 +5159,7 @@
       <c r="AK41" s="46"/>
       <c r="AL41" s="46"/>
     </row>
-    <row r="42" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="39" t="s">
         <v>47</v>
       </c>
@@ -5262,7 +5249,7 @@
       <c r="AK42" s="46"/>
       <c r="AL42" s="46"/>
     </row>
-    <row r="43" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A43" s="39" t="s">
         <v>48</v>
       </c>
@@ -5352,7 +5339,7 @@
       <c r="AK43" s="66"/>
       <c r="AL43" s="66"/>
     </row>
-    <row r="44" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A44" s="39" t="s">
         <v>46</v>
       </c>
@@ -5442,7 +5429,7 @@
       <c r="AK44" s="46"/>
       <c r="AL44" s="46"/>
     </row>
-    <row r="45" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A45" s="39" t="s">
         <v>45</v>
       </c>
@@ -5532,7 +5519,7 @@
       <c r="AK45" s="46"/>
       <c r="AL45" s="46"/>
     </row>
-    <row r="46" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>51</v>
       </c>
@@ -5622,7 +5609,7 @@
       <c r="AK46" s="46"/>
       <c r="AL46" s="46"/>
     </row>
-    <row r="47" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>52</v>
       </c>
@@ -5712,7 +5699,7 @@
       <c r="AK47" s="46"/>
       <c r="AL47" s="46"/>
     </row>
-    <row r="48" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>49</v>
       </c>
@@ -5802,7 +5789,7 @@
       <c r="AK48" s="46"/>
       <c r="AL48" s="46"/>
     </row>
-    <row r="49" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="73" t="s">
         <v>50</v>
       </c>
@@ -5892,7 +5879,7 @@
       <c r="AK49" s="46"/>
       <c r="AL49" s="46"/>
     </row>
-    <row r="50" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="88" t="s">
         <v>12</v>
       </c>
@@ -6004,7 +5991,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="51" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="87" t="s">
         <v>17</v>
       </c>
@@ -6112,7 +6099,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="52" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="87" t="s">
         <v>16</v>
       </c>
@@ -6220,7 +6207,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="53" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="87" t="s">
         <v>23</v>
       </c>
@@ -6332,7 +6319,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="87" t="s">
         <v>29</v>
       </c>
@@ -6444,7 +6431,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="55" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A55" s="87" t="s">
         <v>42</v>
       </c>
@@ -6556,7 +6543,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="56" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="87" t="s">
         <v>31</v>
       </c>
@@ -6668,7 +6655,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="57" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="87" t="s">
         <v>37</v>
       </c>
@@ -6780,7 +6767,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="94" t="s">
         <v>12</v>
       </c>
@@ -6823,7 +6810,7 @@
         <v>2</v>
       </c>
       <c r="P58" s="95" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="Q58" s="94" t="s">
         <v>16</v>
@@ -6892,7 +6879,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="59" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A59" s="84" t="s">
         <v>29</v>
       </c>
@@ -7004,7 +6991,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="60" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="84" t="s">
         <v>9</v>
       </c>
@@ -7116,7 +7103,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="61" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A61" s="84" t="s">
         <v>31</v>
       </c>
@@ -7228,7 +7215,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="62" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="104" t="s">
         <v>17</v>
       </c>
@@ -7340,7 +7327,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="63" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="84" t="s">
         <v>23</v>
       </c>
@@ -7452,12 +7439,12 @@
         <v>27</v>
       </c>
     </row>
-    <row r="64" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:38" s="96" customFormat="1" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="94" t="s">
-        <v>94</v>
+        <v>42</v>
       </c>
       <c r="B64" s="94" t="s">
-        <v>95</v>
+        <v>36</v>
       </c>
       <c r="C64" s="89">
         <v>43295</v>
@@ -7468,21 +7455,35 @@
       <c r="E64" s="91">
         <v>0.66666666666666663</v>
       </c>
-      <c r="F64" s="92"/>
-      <c r="G64" s="92"/>
-      <c r="H64" s="92"/>
+      <c r="F64" s="92">
+        <v>2.2200000000000002</v>
+      </c>
+      <c r="G64" s="92">
+        <v>3.75</v>
+      </c>
+      <c r="H64" s="92">
+        <v>3.4</v>
+      </c>
       <c r="I64" s="92"/>
       <c r="J64" s="92"/>
-      <c r="K64" s="92"/>
-      <c r="L64" s="93"/>
+      <c r="K64" s="92">
+        <v>1</v>
+      </c>
+      <c r="L64" s="93" t="s">
+        <v>73</v>
+      </c>
       <c r="M64" s="94" t="s">
         <v>12</v>
       </c>
       <c r="N64" s="94" t="s">
         <v>23</v>
       </c>
-      <c r="O64" s="92"/>
-      <c r="P64" s="95"/>
+      <c r="O64" s="92" t="s">
+        <v>58</v>
+      </c>
+      <c r="P64" s="95" t="s">
+        <v>68</v>
+      </c>
       <c r="Q64" s="94" t="s">
         <v>16</v>
       </c>
@@ -7497,8 +7498,12 @@
       <c r="V64" s="94" t="s">
         <v>15</v>
       </c>
-      <c r="W64" s="92"/>
-      <c r="X64" s="95"/>
+      <c r="W64" s="92">
+        <v>1</v>
+      </c>
+      <c r="X64" s="95" t="s">
+        <v>73</v>
+      </c>
       <c r="Y64" s="94" t="s">
         <v>29</v>
       </c>
@@ -7530,12 +7535,12 @@
         <v>15</v>
       </c>
     </row>
-    <row r="65" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="84" t="s">
-        <v>96</v>
+        <v>17</v>
       </c>
       <c r="B65" s="84" t="s">
-        <v>97</v>
+        <v>23</v>
       </c>
       <c r="C65" s="34">
         <v>43296</v>
@@ -7546,21 +7551,35 @@
       <c r="E65" s="38">
         <v>0.70833333333333337</v>
       </c>
-      <c r="F65" s="22"/>
-      <c r="G65" s="22"/>
-      <c r="H65" s="22"/>
+      <c r="F65" s="22">
+        <v>1.9</v>
+      </c>
+      <c r="G65" s="22">
+        <v>3.3</v>
+      </c>
+      <c r="H65" s="22">
+        <v>5</v>
+      </c>
       <c r="I65" s="24"/>
       <c r="J65" s="24"/>
-      <c r="K65" s="16"/>
-      <c r="L65" s="46"/>
+      <c r="K65" s="16">
+        <v>2</v>
+      </c>
+      <c r="L65" s="46" t="s">
+        <v>70</v>
+      </c>
       <c r="M65" s="82" t="s">
         <v>27</v>
       </c>
       <c r="N65" s="82" t="s">
         <v>42</v>
       </c>
-      <c r="O65" s="19"/>
-      <c r="P65" s="81"/>
+      <c r="O65" s="19">
+        <v>1</v>
+      </c>
+      <c r="P65" s="81" t="s">
+        <v>75</v>
+      </c>
       <c r="Q65" s="83" t="s">
         <v>42</v>
       </c>
@@ -7575,8 +7594,12 @@
       <c r="V65" s="82" t="s">
         <v>27</v>
       </c>
-      <c r="W65" s="19"/>
-      <c r="X65" s="81"/>
+      <c r="W65" s="19">
+        <v>1</v>
+      </c>
+      <c r="X65" s="81" t="s">
+        <v>69</v>
+      </c>
       <c r="Y65" s="83" t="s">
         <v>15</v>
       </c>
@@ -7608,777 +7631,777 @@
         <v>27</v>
       </c>
     </row>
-    <row r="66" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="67" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="68" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="69" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="70" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="71" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="72" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="73" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="74" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="75" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="76" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="77" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="78" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="79" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="80" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
-    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
+    <row r="66" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="67" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="68" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="69" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="70" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="71" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="72" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="73" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="74" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="75" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="76" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="77" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="78" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="79" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="80" spans="1:38" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="81" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="82" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="83" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="84" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="85" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="86" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="87" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="88" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="89" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="90" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="91" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="92" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="93" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="94" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="95" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="96" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="97" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="98" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="99" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="100" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="101" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="102" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="103" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="104" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="105" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="106" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="107" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="108" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="109" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="110" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="111" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="112" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="113" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="114" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="115" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="116" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="117" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="118" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="119" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="120" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="121" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="122" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="123" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="124" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="125" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="126" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="127" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="128" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="129" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="130" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="131" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="132" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="133" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="134" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="135" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="136" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="137" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="138" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="139" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="140" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="141" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="142" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="143" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="144" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="145" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="146" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="147" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="148" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="149" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="150" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="151" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="152" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="153" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="154" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="155" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="156" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="157" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="158" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="159" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="160" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="161" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="162" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="163" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="164" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="165" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="166" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="167" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="168" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="169" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="170" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="171" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="172" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="173" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="174" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="175" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="176" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="177" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="178" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="179" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="180" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="181" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="182" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="183" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="184" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="185" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="186" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="187" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="188" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="189" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="190" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="191" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="192" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="193" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="194" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="195" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="196" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="197" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="198" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="199" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="200" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="201" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="202" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="203" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="204" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="205" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="206" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="207" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="208" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="209" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="210" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="211" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="212" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="213" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="214" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="215" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="216" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="217" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="218" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="219" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="220" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="221" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="222" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="223" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="224" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="225" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="226" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="227" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="228" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="229" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="230" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="231" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="232" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="233" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="234" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="235" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="236" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="237" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="238" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="239" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="240" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="241" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="242" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="243" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="244" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="245" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="246" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="247" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="248" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="249" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="250" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="251" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="252" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="253" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="254" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="255" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="256" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="257" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="258" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="259" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="260" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="261" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="262" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="263" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="264" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="265" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="266" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="267" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="268" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="269" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="270" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="271" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="272" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="273" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="274" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="275" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="276" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="277" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="278" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="279" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="280" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="281" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="282" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="283" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="284" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="285" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="286" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="287" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="288" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="289" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="290" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="291" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="292" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="293" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="294" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="295" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="296" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="297" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="298" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="299" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="300" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="301" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="302" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="303" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="304" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="305" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="306" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="307" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="308" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="309" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="310" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="311" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="312" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="313" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="314" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="315" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="316" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="317" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="318" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="319" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="320" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="321" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="322" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="323" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="324" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="325" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="326" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="327" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="328" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="329" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="330" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="331" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="332" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="333" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="334" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="335" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="336" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="337" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="338" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="339" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="340" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="341" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="342" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="343" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="344" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="345" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="346" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="347" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="348" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="349" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="350" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="351" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="352" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="353" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="354" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="355" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="356" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="357" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="358" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="359" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="360" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="361" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="362" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="363" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="364" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="365" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="366" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="367" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="368" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="369" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="370" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="371" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="372" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="373" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="374" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="375" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="376" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="377" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="378" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="379" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="380" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="381" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="382" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="383" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="384" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="385" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="386" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="387" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="388" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="389" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="390" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="391" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="392" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="393" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="394" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="395" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="396" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="397" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="398" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="399" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="400" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="401" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="402" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="403" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="404" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="405" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="406" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="407" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="408" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="409" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="410" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="411" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="412" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="413" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="414" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="415" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="416" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="417" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="418" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="419" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="420" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="421" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="422" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="423" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="424" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="425" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="426" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="427" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="428" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="429" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="430" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="431" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="432" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="433" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="434" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="435" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="436" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="437" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="438" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="439" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="440" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="441" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="442" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="443" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="444" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="445" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="446" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="447" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="448" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="449" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="450" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="451" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="452" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="453" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="454" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="455" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="456" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="457" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="458" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="459" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="460" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="461" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="462" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="463" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="464" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="465" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="466" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="467" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="468" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="469" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="470" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="471" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="472" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="473" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="474" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="475" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="476" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="477" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="478" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="479" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="480" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="481" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="482" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="483" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="484" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="485" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="486" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="487" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="488" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="489" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="490" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="491" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="492" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="493" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="494" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="495" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="496" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="497" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="498" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="499" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="500" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="501" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="502" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="503" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="504" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="505" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="506" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="507" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="508" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="509" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="510" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="511" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="512" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="513" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="514" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="515" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="516" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="517" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="518" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="519" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="520" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="521" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="522" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="523" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="524" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="525" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="526" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="527" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="528" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="529" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="530" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="531" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="532" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="533" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="534" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="535" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="536" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="537" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="538" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="539" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="540" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="541" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="542" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="543" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="544" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="545" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="546" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="547" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="548" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="549" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="550" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="551" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="552" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="553" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="554" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="555" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="556" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="557" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="558" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="559" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="560" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="561" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="562" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="563" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="564" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="565" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="566" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="567" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="568" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="569" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="570" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="571" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="572" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="573" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="574" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="575" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="576" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="577" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="578" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="579" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="580" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="581" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="582" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="583" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="584" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="585" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="586" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="587" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="588" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="589" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="590" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="591" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="592" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="593" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="594" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="595" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="596" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="597" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="598" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="599" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="600" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="601" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="602" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="603" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="604" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="605" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="606" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="607" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="608" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="609" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="610" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="611" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="612" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="613" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="614" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="615" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="616" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="617" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="618" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="619" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="620" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="621" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="622" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="623" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="624" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="625" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="626" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="627" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="628" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="629" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="630" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="631" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="632" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="633" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="634" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="635" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="636" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="637" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="638" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="639" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="640" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="641" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="642" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="643" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="644" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="645" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="646" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="647" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="648" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="649" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="650" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="651" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="652" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="653" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="654" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="655" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="656" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="657" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="658" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="659" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="660" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="661" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="662" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="663" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="664" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="665" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="666" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="667" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="668" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="669" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="670" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="671" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="672" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="673" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="674" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="675" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="676" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="677" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="678" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="679" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="680" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="681" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="682" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="683" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="684" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="685" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="686" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="687" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="688" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="689" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="690" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="691" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="692" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="693" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="694" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="695" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="696" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="697" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="698" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="699" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="700" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="701" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="702" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="703" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="704" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="705" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="706" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="707" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="708" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="709" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="710" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="711" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="712" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="713" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="714" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="715" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="716" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="717" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="718" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="719" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="720" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="721" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="722" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="723" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="724" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="725" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="726" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="727" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="728" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="729" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="730" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="731" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="732" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="733" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="734" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="735" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="736" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="737" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="738" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="739" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="740" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="741" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="742" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="743" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="744" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="745" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="746" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="747" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="748" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="749" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="750" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="751" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="752" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="753" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="754" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="755" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="756" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="757" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="758" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="759" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="760" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="761" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="762" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="763" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="764" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="765" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="766" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="767" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="768" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="769" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="770" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="771" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="772" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="773" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="774" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="775" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="776" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="777" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="778" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="779" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="780" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="781" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="782" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="783" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="784" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="785" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="786" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="787" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="788" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="789" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="790" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="791" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="792" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="793" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="794" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="795" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="796" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="797" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="798" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="799" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="800" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="801" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="802" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="803" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="804" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="805" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="806" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="807" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="808" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="809" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="810" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="811" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="812" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="813" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="814" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="815" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="816" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="817" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="818" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="819" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="820" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="821" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="822" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="823" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="824" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="825" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="826" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="827" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="828" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="829" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="830" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="831" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="832" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="833" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="834" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="835" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="836" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -8389,16 +8412,16 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:K50"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="M25" sqref="M25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C1" s="105" t="s">
         <v>55</v>
       </c>
@@ -8408,7 +8431,7 @@
       </c>
       <c r="F1" s="106"/>
     </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>1</v>
       </c>
@@ -8437,7 +8460,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="11" t="s">
         <v>9</v>
       </c>
@@ -8477,7 +8500,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A4" s="11" t="s">
         <v>11</v>
       </c>
@@ -8517,7 +8540,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="11" t="s">
         <v>15</v>
       </c>
@@ -8557,7 +8580,7 @@
         <v>2.2999999999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="11" t="s">
         <v>13</v>
       </c>
@@ -8597,7 +8620,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="7" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="11" t="s">
         <v>17</v>
       </c>
@@ -8637,7 +8660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="11" t="s">
         <v>21</v>
       </c>
@@ -8677,7 +8700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A9" s="11" t="s">
         <v>19</v>
       </c>
@@ -8717,7 +8740,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="10" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="11" t="s">
         <v>23</v>
       </c>
@@ -8757,7 +8780,7 @@
         <v>2.1</v>
       </c>
     </row>
-    <row r="11" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="11" t="s">
         <v>29</v>
       </c>
@@ -8797,7 +8820,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="12" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A12" s="11" t="s">
         <v>25</v>
       </c>
@@ -8837,7 +8860,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="13" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A13" s="11" t="s">
         <v>27</v>
       </c>
@@ -8877,7 +8900,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="14" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="9" t="s">
         <v>31</v>
       </c>
@@ -8917,7 +8940,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A15" s="9" t="s">
         <v>33</v>
       </c>
@@ -8957,7 +8980,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A16" s="9" t="s">
         <v>35</v>
       </c>
@@ -8997,7 +9020,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="11" t="s">
         <v>39</v>
       </c>
@@ -9037,7 +9060,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="18" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="11" t="s">
         <v>37</v>
       </c>
@@ -9077,7 +9100,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="19" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A19" s="11" t="s">
         <v>9</v>
       </c>
@@ -9117,7 +9140,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="20" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="11" t="s">
         <v>12</v>
       </c>
@@ -9157,7 +9180,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="21" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="11" t="s">
         <v>15</v>
       </c>
@@ -9197,7 +9220,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A22" s="11" t="s">
         <v>41</v>
       </c>
@@ -9237,7 +9260,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A23" s="11" t="s">
         <v>17</v>
       </c>
@@ -9277,7 +9300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A24" s="11" t="s">
         <v>22</v>
       </c>
@@ -9317,7 +9340,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="25" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A25" s="11" t="s">
         <v>19</v>
       </c>
@@ -9357,7 +9380,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="26" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A26" s="11" t="s">
         <v>24</v>
       </c>
@@ -9397,7 +9420,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="27" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A27" s="11" t="s">
         <v>29</v>
       </c>
@@ -9437,7 +9460,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="28" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="11" t="s">
         <v>26</v>
       </c>
@@ -9477,7 +9500,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="29" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A29" s="11" t="s">
         <v>27</v>
       </c>
@@ -9517,7 +9540,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A30" s="11" t="s">
         <v>32</v>
       </c>
@@ -9557,7 +9580,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="31" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A31" s="11" t="s">
         <v>42</v>
       </c>
@@ -9597,7 +9620,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="11" t="s">
         <v>36</v>
       </c>
@@ -9637,7 +9660,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="33" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="11" t="s">
         <v>43</v>
       </c>
@@ -9677,7 +9700,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A34" s="11" t="s">
         <v>38</v>
       </c>
@@ -9717,7 +9740,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="35" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="11" t="s">
         <v>12</v>
       </c>
@@ -9757,7 +9780,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="36" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A36" s="11" t="s">
         <v>10</v>
       </c>
@@ -9797,7 +9820,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A37" s="9" t="s">
         <v>14</v>
       </c>
@@ -9837,7 +9860,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="38" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A38" s="9" t="s">
         <v>16</v>
       </c>
@@ -9877,7 +9900,7 @@
         <v>1.8</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A39" s="11" t="s">
         <v>22</v>
       </c>
@@ -9917,7 +9940,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A40" s="11" t="s">
         <v>18</v>
       </c>
@@ -9957,7 +9980,7 @@
         <v>1.9</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A41" s="11" t="s">
         <v>44</v>
       </c>
@@ -9997,7 +10020,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A42" s="11" t="s">
         <v>20</v>
       </c>
@@ -10037,7 +10060,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="43" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A43" s="11" t="s">
         <v>47</v>
       </c>
@@ -10077,7 +10100,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="44" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A44" s="11" t="s">
         <v>48</v>
       </c>
@@ -10117,7 +10140,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A45" s="11" t="s">
         <v>46</v>
       </c>
@@ -10157,7 +10180,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A46" s="11" t="s">
         <v>45</v>
       </c>
@@ -10197,7 +10220,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="47" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A47" s="11" t="s">
         <v>51</v>
       </c>
@@ -10237,7 +10260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="48" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A48" s="11" t="s">
         <v>52</v>
       </c>
@@ -10277,7 +10300,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="49" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A49" s="11" t="s">
         <v>49</v>
       </c>
@@ -10317,7 +10340,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="50" spans="1:11" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:11" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A50" s="11" t="s">
         <v>50</v>
       </c>
@@ -10367,7 +10390,7 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
@@ -10377,9 +10400,9 @@
       <selection activeCell="J13" sqref="J13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="14.5" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C3" t="s">
         <v>56</v>
       </c>
@@ -10387,12 +10410,12 @@
       <c r="J3" s="7"/>
       <c r="K3" s="7"/>
     </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
       <c r="I4" s="7"/>
       <c r="J4" s="7"/>
       <c r="K4" s="7"/>
     </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="C5" s="4">
         <v>1</v>
       </c>
@@ -10406,7 +10429,7 @@
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
     </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A6" s="11" t="s">
         <v>9</v>
       </c>
@@ -10426,7 +10449,7 @@
       <c r="J6" s="7"/>
       <c r="K6" s="7"/>
     </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A7" s="11" t="s">
         <v>11</v>
       </c>
@@ -10446,7 +10469,7 @@
       <c r="J7" s="7"/>
       <c r="K7" s="7"/>
     </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" s="11" t="s">
         <v>15</v>
       </c>
@@ -10466,7 +10489,7 @@
       <c r="J8" s="7"/>
       <c r="K8" s="7"/>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" s="11" t="s">
         <v>13</v>
       </c>
@@ -10486,7 +10509,7 @@
       <c r="J9" s="7"/>
       <c r="K9" s="7"/>
     </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" s="11" t="s">
         <v>17</v>
       </c>
@@ -10506,7 +10529,7 @@
       <c r="J10" s="7"/>
       <c r="K10" s="7"/>
     </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
@@ -10526,7 +10549,7 @@
       <c r="J11" s="7"/>
       <c r="K11" s="7"/>
     </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" s="11" t="s">
         <v>19</v>
       </c>
@@ -10546,7 +10569,7 @@
       <c r="J12" s="7"/>
       <c r="K12" s="7"/>
     </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" s="11" t="s">
         <v>23</v>
       </c>
@@ -10568,7 +10591,7 @@
       </c>
       <c r="K13" s="7"/>
     </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" s="11" t="s">
         <v>29</v>
       </c>
@@ -10588,7 +10611,7 @@
       <c r="J14" s="7"/>
       <c r="K14" s="7"/>
     </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" s="11" t="s">
         <v>25</v>
       </c>
@@ -10608,7 +10631,7 @@
       <c r="J15" s="7"/>
       <c r="K15" s="7"/>
     </row>
-    <row r="16" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A16" s="11" t="s">
         <v>27</v>
       </c>
@@ -10628,7 +10651,7 @@
       <c r="J16" s="7"/>
       <c r="K16" s="7"/>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" s="9" t="s">
         <v>31</v>
       </c>
@@ -10648,7 +10671,7 @@
       <c r="J17" s="7"/>
       <c r="K17" s="7"/>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A18" s="9" t="s">
         <v>33</v>
       </c>
@@ -10668,7 +10691,7 @@
       <c r="J18" s="7"/>
       <c r="K18" s="7"/>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" s="9" t="s">
         <v>35</v>
       </c>
@@ -10688,7 +10711,7 @@
       <c r="J19" s="7"/>
       <c r="K19" s="7"/>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" s="11" t="s">
         <v>39</v>
       </c>
@@ -10708,7 +10731,7 @@
       <c r="J20" s="7"/>
       <c r="K20" s="7"/>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" s="11" t="s">
         <v>37</v>
       </c>
@@ -10728,7 +10751,7 @@
       <c r="J21" s="7"/>
       <c r="K21" s="7"/>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" s="11" t="s">
         <v>9</v>
       </c>
@@ -10748,7 +10771,7 @@
       <c r="J22" s="7"/>
       <c r="K22" s="7"/>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" s="11" t="s">
         <v>12</v>
       </c>
@@ -10768,7 +10791,7 @@
       <c r="J23" s="7"/>
       <c r="K23" s="7"/>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" s="11" t="s">
         <v>15</v>
       </c>
@@ -10788,7 +10811,7 @@
       <c r="J24" s="7"/>
       <c r="K24" s="7"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" s="11" t="s">
         <v>41</v>
       </c>
@@ -10808,7 +10831,7 @@
       <c r="J25" s="7"/>
       <c r="K25" s="7"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" s="11" t="s">
         <v>17</v>
       </c>
@@ -10828,7 +10851,7 @@
       <c r="J26" s="7"/>
       <c r="K26" s="7"/>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A27" s="11" t="s">
         <v>22</v>
       </c>
@@ -10848,7 +10871,7 @@
       <c r="J27" s="7"/>
       <c r="K27" s="7"/>
     </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" s="11" t="s">
         <v>19</v>
       </c>
@@ -10868,7 +10891,7 @@
       <c r="J28" s="7"/>
       <c r="K28" s="7"/>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A29" s="11" t="s">
         <v>24</v>
       </c>
@@ -10888,7 +10911,7 @@
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" s="11" t="s">
         <v>29</v>
       </c>
@@ -10908,7 +10931,7 @@
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
     </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A31" s="11" t="s">
         <v>26</v>
       </c>
@@ -10928,7 +10951,7 @@
       <c r="J31" s="7"/>
       <c r="K31" s="7"/>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" s="11" t="s">
         <v>27</v>
       </c>
@@ -10948,7 +10971,7 @@
       <c r="J32" s="7"/>
       <c r="K32" s="7"/>
     </row>
-    <row r="33" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" s="11" t="s">
         <v>32</v>
       </c>
@@ -10968,7 +10991,7 @@
       <c r="J33" s="7"/>
       <c r="K33" s="7"/>
     </row>
-    <row r="34" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" s="11" t="s">
         <v>42</v>
       </c>
@@ -10988,7 +11011,7 @@
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
     </row>
-    <row r="35" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A35" s="11" t="s">
         <v>36</v>
       </c>
@@ -11008,7 +11031,7 @@
       <c r="J35" s="7"/>
       <c r="K35" s="7"/>
     </row>
-    <row r="36" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A36" s="11" t="s">
         <v>43</v>
       </c>
@@ -11028,7 +11051,7 @@
       <c r="J36" s="7"/>
       <c r="K36" s="7"/>
     </row>
-    <row r="37" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A37" s="11" t="s">
         <v>38</v>
       </c>
@@ -11048,7 +11071,7 @@
       <c r="J37" s="7"/>
       <c r="K37" s="7"/>
     </row>
-    <row r="38" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A38" s="11" t="s">
         <v>12</v>
       </c>
@@ -11068,7 +11091,7 @@
       <c r="J38" s="7"/>
       <c r="K38" s="7"/>
     </row>
-    <row r="39" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A39" s="11" t="s">
         <v>10</v>
       </c>
@@ -11088,7 +11111,7 @@
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
     </row>
-    <row r="40" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A40" s="9" t="s">
         <v>14</v>
       </c>
@@ -11108,7 +11131,7 @@
       <c r="J40" s="7"/>
       <c r="K40" s="7"/>
     </row>
-    <row r="41" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A41" s="9" t="s">
         <v>16</v>
       </c>
@@ -11128,7 +11151,7 @@
       <c r="J41" s="7"/>
       <c r="K41" s="7"/>
     </row>
-    <row r="42" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A42" s="11" t="s">
         <v>22</v>
       </c>
@@ -11148,7 +11171,7 @@
       <c r="J42" s="7"/>
       <c r="K42" s="7"/>
     </row>
-    <row r="43" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A43" s="11" t="s">
         <v>18</v>
       </c>
@@ -11168,7 +11191,7 @@
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
     </row>
-    <row r="44" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A44" s="11" t="s">
         <v>44</v>
       </c>
@@ -11188,7 +11211,7 @@
       <c r="J44" s="7"/>
       <c r="K44" s="7"/>
     </row>
-    <row r="45" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A45" s="11" t="s">
         <v>20</v>
       </c>
@@ -11208,7 +11231,7 @@
       <c r="J45" s="7"/>
       <c r="K45" s="7"/>
     </row>
-    <row r="46" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A46" s="11" t="s">
         <v>47</v>
       </c>
@@ -11228,7 +11251,7 @@
       <c r="J46" s="7"/>
       <c r="K46" s="7"/>
     </row>
-    <row r="47" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A47" s="11" t="s">
         <v>48</v>
       </c>
@@ -11248,7 +11271,7 @@
       <c r="J47" s="7"/>
       <c r="K47" s="7"/>
     </row>
-    <row r="48" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A48" s="11" t="s">
         <v>46</v>
       </c>
@@ -11268,7 +11291,7 @@
       <c r="J48" s="7"/>
       <c r="K48" s="7"/>
     </row>
-    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A49" s="11" t="s">
         <v>45</v>
       </c>
@@ -11288,7 +11311,7 @@
       <c r="J49" s="7"/>
       <c r="K49" s="7"/>
     </row>
-    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A50" s="11" t="s">
         <v>51</v>
       </c>
@@ -11308,7 +11331,7 @@
       <c r="J50" s="7"/>
       <c r="K50" s="7"/>
     </row>
-    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="11" t="s">
         <v>52</v>
       </c>
@@ -11325,7 +11348,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A52" s="11" t="s">
         <v>49</v>
       </c>
@@ -11342,7 +11365,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:11" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A53" s="11" t="s">
         <v>50</v>
       </c>

</xml_diff>